<commit_message>
Mise à jour fichier test et fichier en PDF
</commit_message>
<xml_diff>
--- a/Dossier_Conception/Jeux de test.xlsx
+++ b/Dossier_Conception/Jeux de test.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b0765a34999f590/Eclipse3/CalculatriceV2/Dossier_Conception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{02729F76-CAF2-475A-AC88-482CF607712C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E97BB66B-87BA-4245-828E-0117AD1B3511}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{02729F76-CAF2-475A-AC88-482CF607712C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D6420E94-6E5A-4CFD-B0FC-ACADEFFD2B66}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-1965" windowWidth="25440" windowHeight="15390" xr2:uid="{602560AE-A1EC-4A49-9DE1-3327F717E989}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$B$65</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Saisies</t>
   </si>
@@ -42,16 +45,10 @@
     <t xml:space="preserve">L'addition </t>
   </si>
   <si>
-    <t>91.2</t>
-  </si>
-  <si>
     <t>Saisie décimale</t>
   </si>
   <si>
     <t>.36</t>
-  </si>
-  <si>
-    <t>0.36</t>
   </si>
   <si>
     <t>2369.123852</t>
@@ -107,15 +104,9 @@
     <t>24.36 + 98,65 (+/-) =</t>
   </si>
   <si>
-    <t>-74.29</t>
-  </si>
-  <si>
     <t>12.3 (+/-) + 0.54 (+/-) =</t>
   </si>
   <si>
-    <t>-12.84</t>
-  </si>
-  <si>
     <t>Trop Grand</t>
   </si>
   <si>
@@ -131,15 +122,9 @@
     <t>456.369 - 74.89 =</t>
   </si>
   <si>
-    <t>381.479</t>
-  </si>
-  <si>
     <t xml:space="preserve">45.2 (+/-) - 84,6 = </t>
   </si>
   <si>
-    <t>-129.8</t>
-  </si>
-  <si>
     <t>12 (+/-) - 41 (+/-) =</t>
   </si>
   <si>
@@ -152,24 +137,15 @@
     <t xml:space="preserve">45.5698 x 74.4126 = </t>
   </si>
   <si>
-    <t>3390.967299</t>
-  </si>
-  <si>
     <t xml:space="preserve">78.3 (+/-) x .85 = </t>
   </si>
   <si>
-    <t>-66.555</t>
-  </si>
-  <si>
     <t>14 (+/-) x 91 (+/-) =</t>
   </si>
   <si>
     <t xml:space="preserve">0.856942365 x .8945136364 = </t>
   </si>
   <si>
-    <t>0.7665466311</t>
-  </si>
-  <si>
     <t xml:space="preserve">987654321 x 951951951 = </t>
   </si>
   <si>
@@ -182,27 +158,15 @@
     <t xml:space="preserve">78.1596 / 41.23 = </t>
   </si>
   <si>
-    <t>1.895697308</t>
-  </si>
-  <si>
     <t>63.425 / .36 =</t>
   </si>
   <si>
-    <t>176.1805556</t>
-  </si>
-  <si>
     <t xml:space="preserve">62,5 (+/-) / 3.47 = </t>
   </si>
   <si>
-    <t>-18.01152738</t>
-  </si>
-  <si>
     <t xml:space="preserve">89 / 12.36 (+/-) = </t>
   </si>
   <si>
-    <t>-7.200647249</t>
-  </si>
-  <si>
     <t xml:space="preserve">.456 (+/-) / 52.147 (+/-) = </t>
   </si>
   <si>
@@ -212,21 +176,12 @@
     <t>/ par 0</t>
   </si>
   <si>
-    <t>12.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">.21 * 5.6 + 4 = </t>
   </si>
   <si>
-    <t>5.176</t>
-  </si>
-  <si>
     <t>6 + 3 - 4 x 5 / 2 =</t>
   </si>
   <si>
-    <t>-3.69230692</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.2 (+/-) x 3 / 2.6 = </t>
   </si>
   <si>
@@ -242,24 +197,15 @@
     <t>56.36 √</t>
   </si>
   <si>
-    <t>7.50733</t>
-  </si>
-  <si>
     <t>48 (+/-) √</t>
   </si>
   <si>
     <t>Erreur</t>
   </si>
   <si>
-    <t>0.03</t>
-  </si>
-  <si>
     <t>456.852 %</t>
   </si>
   <si>
-    <t>4.56852</t>
-  </si>
-  <si>
     <t>Le pourcent</t>
   </si>
   <si>
@@ -275,20 +221,44 @@
     <t>41.56 - 12.75 = (M+) 85 + 12 = (M-)  (MRC)</t>
   </si>
   <si>
-    <t>28.81 et 97 et -68.19</t>
-  </si>
-  <si>
-    <t>-68.19 et 0</t>
-  </si>
-  <si>
     <t>(MRC) (M-) (MRC)</t>
+  </si>
+  <si>
+    <t>Test Calculatrice</t>
+  </si>
+  <si>
+    <t>-74,29</t>
+  </si>
+  <si>
+    <t>-12,84</t>
+  </si>
+  <si>
+    <t>-129,8</t>
+  </si>
+  <si>
+    <t>-66,555</t>
+  </si>
+  <si>
+    <t>-18,01152738</t>
+  </si>
+  <si>
+    <t>-7,200647249</t>
+  </si>
+  <si>
+    <t>-3,69230692</t>
+  </si>
+  <si>
+    <t>28,81 et 97 et -68,19</t>
+  </si>
+  <si>
+    <t>-68,19 et 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +282,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -321,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -329,11 +315,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,20 +342,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E97CA8F-F02F-4BD0-A4FE-8F51EC7B06E4}">
-  <dimension ref="A2:B65"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,6 +687,12 @@
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
@@ -691,422 +702,423 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2369.1238520000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B15" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" s="7">
+        <v>91.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" s="6">
+        <v>1201259745</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>1201259745</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" s="6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" s="6">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="5"/>
+      <c r="A24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6">
+        <v>-82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="7">
+        <v>381.47899999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B29" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>-82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B32" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B33" s="7">
+        <v>3390.9672989999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B34" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B35" s="6">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B36" s="7">
+        <v>0.76654663109999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B37" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1.8956973079999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="7">
+        <v>176.18055559999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B46" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="7">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40">
+      <c r="B50" s="7">
+        <v>5.1760000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B55" s="7">
+        <v>7.5073299999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B56" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="4" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="B59" s="7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B60" s="7">
+        <v>4.5685200000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="5"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B64" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="5"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>63</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="3" t="s">
+      <c r="B65" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="5"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" s="5"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>